<commit_message>
Updated scenarios and sensitivities spreadsheet
</commit_message>
<xml_diff>
--- a/Scenarios_Sensitivities.xlsx
+++ b/Scenarios_Sensitivities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SWITCH\india_ED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Electricity_Models\renewable_energy_value\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +505,7 @@
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
archiving net_load_hydro outputs and conventional generation buildout outputs to RE integration conference folder. These outputs might change when net load is estimated with lookahead period
</commit_message>
<xml_diff>
--- a/Scenarios_Sensitivities.xlsx
+++ b/Scenarios_Sensitivities.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Scenarios</t>
   </si>
@@ -95,12 +96,6 @@
     <t>Nuclear 64 GW</t>
   </si>
   <si>
-    <t>Battery Storage 5% daily energy</t>
-  </si>
-  <si>
-    <t>Battery Storage 10% daily energy</t>
-  </si>
-  <si>
     <t>Demand response 5% daily energy</t>
   </si>
   <si>
@@ -162,6 +157,117 @@
   </si>
   <si>
     <t>55min</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>add FGD and other adders from CEA report</t>
+  </si>
+  <si>
+    <t>Battery Storage 20% peak ~ 60 GW</t>
+  </si>
+  <si>
+    <t>Battery Storage 10% peak ~ 30 GW</t>
+  </si>
+  <si>
+    <t>Battery Storage 15% peak ~ 45 GW</t>
+  </si>
+  <si>
+    <t>Battery Storage 5% peak ~ 15 GW</t>
+  </si>
+  <si>
+    <t>CANCEL; just compare DR to storage in text. Storage efficiency, which leads to additional energy for charging is akin to DR rebound whre consumption may increase in non-peak hours.</t>
+  </si>
+  <si>
+    <t>CANCEL?</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>I don't have capacity costs for nuclear. Can only determine energy value</t>
+  </si>
+  <si>
+    <t>stobat15</t>
+  </si>
+  <si>
+    <t>stobat30</t>
+  </si>
+  <si>
+    <t>stobat45</t>
+  </si>
+  <si>
+    <t>stobat60</t>
+  </si>
+  <si>
+    <t>nuc64</t>
+  </si>
+  <si>
+    <t>hydroHE25p</t>
+  </si>
+  <si>
+    <t>hydroLE25p</t>
+  </si>
+  <si>
+    <t>high energy</t>
+  </si>
+  <si>
+    <t>low energy</t>
+  </si>
+  <si>
+    <t>Wind 100m HH</t>
+  </si>
+  <si>
+    <t>Wind 120m HH</t>
+  </si>
+  <si>
+    <t>Solar 1axis tracking</t>
+  </si>
+  <si>
+    <t>Solar 45deg Southwest</t>
+  </si>
+  <si>
+    <t>Solar 90deg West</t>
+  </si>
+  <si>
+    <t>that's 15% of solar 200 GW target</t>
+  </si>
+  <si>
+    <t>that's 30% of solar 200 GW target</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>screening curve</t>
+  </si>
+  <si>
+    <t>econ dispatch script</t>
+  </si>
+  <si>
+    <t>R script</t>
+  </si>
+  <si>
+    <t>input file with extension</t>
+  </si>
+  <si>
+    <t>loadMod2014</t>
+  </si>
+  <si>
+    <t>wind100</t>
+  </si>
+  <si>
+    <t>wind120</t>
+  </si>
+  <si>
+    <t>solar1A</t>
+  </si>
+  <si>
+    <t>solar45deg</t>
+  </si>
+  <si>
+    <t>solar90deg</t>
   </si>
 </sst>
 </file>
@@ -491,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,14 +612,16 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,13 +638,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -547,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>200</v>
       </c>
@@ -555,7 +669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>200</v>
       </c>
@@ -563,7 +677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>200</v>
       </c>
@@ -571,7 +685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>200</v>
       </c>
@@ -579,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>200</v>
       </c>
@@ -587,7 +701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>300</v>
       </c>
@@ -595,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>300</v>
       </c>
@@ -603,7 +717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>300</v>
       </c>
@@ -611,7 +725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>300</v>
       </c>
@@ -619,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>300</v>
       </c>
@@ -627,7 +741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>400</v>
       </c>
@@ -635,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>400</v>
       </c>
@@ -643,7 +757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>400</v>
       </c>
@@ -651,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>400</v>
       </c>
@@ -659,7 +773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>400</v>
       </c>
@@ -667,143 +781,309 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="H26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>18</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>19</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="G31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+      <c r="I33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
+        <v>55</v>
+      </c>
+      <c r="H35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" t="s">
+        <v>56</v>
+      </c>
+      <c r="H36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+      <c r="I38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+      <c r="I39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="F40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+      <c r="I43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>37</v>
+      <c r="I44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>